<commit_message>
Added Sheet5 in data.xlsx with test data
</commit_message>
<xml_diff>
--- a/Institution_Exam_Seating/data.xlsx
+++ b/Institution_Exam_Seating/data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\My_projects\python\Exam_seating_arranger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programming\My_projects\python\Give-My-Seat\Institution_Exam_Seating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123A9794-38A4-4090-9D07-4953B4A14F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5B29B4-F6CF-45A1-971D-3C569B95303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9072" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="allowed_room" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="201">
   <si>
     <t>std_name</t>
   </si>
@@ -2242,8 +2243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B24B53-49A2-40DF-A7A3-221C31C57906}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2381,4 +2382,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA1D2F4-371B-4140-A743-1432FA0069C8}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>